<commit_message>
Usman - users added to run files
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C771124
</commit_message>
<xml_diff>
--- a/PPIUK-FFH/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-FFH/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="208">
   <si>
     <t>UserName</t>
   </si>
@@ -646,7 +646,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,12 +1063,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2641,8 +2642,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2681,13 +2682,7 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>